<commit_message>
add SU2 numeric method and turbulence model SA in chapter 2
</commit_message>
<xml_diff>
--- a/xjh/TEST/AMG_chapter4.xlsx
+++ b/xjh/TEST/AMG_chapter4.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/xjh/thesis/xjh/TEST/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{79FF2480-7A25-914D-8D3D-80C26D09BF9D}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32E6DC7B-ACB2-604A-9409-62DEF1F789EA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1080" yWindow="1460" windowWidth="27440" windowHeight="16040" xr2:uid="{C211C23D-3DF9-AC42-A044-9D51DF0DB045}"/>
   </bookViews>
@@ -680,7 +680,356 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="zh-CN"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:autoTitleDeleted val="1"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.17735192475940506"/>
+          <c:y val="0.10835666375036454"/>
+          <c:w val="0.79209251968503935"/>
+          <c:h val="0.77139617964421114"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:strRef>
+              <c:f>'F4'!$B$30:$D$30</c:f>
+              <c:strCache>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>FGMRES_ILU0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>FGMRES_AMG</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>AMG_ILU</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'F4'!$B$31:$D$31</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>261.32300000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>400.41900000000004</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>460.11900000000003</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-558D-3A4F-88B0-E5BBBCB92250}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="158118368"/>
+        <c:axId val="1855211919"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="158118368"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1855211919"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="1855211919"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US"/>
+                  <a:t>耗时</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>/</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US"/>
+                  <a:t>秒</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="zh-CN"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="95000"/>
+                <a:lumOff val="5000"/>
+              </a:schemeClr>
+            </a:solidFill>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1050" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="zh-CN"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="158118368"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="zh-CN"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
   <a:schemeClr val="accent2"/>
@@ -1236,6 +1585,509 @@
 </cs:chartStyle>
 </file>
 
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -1269,6 +2121,42 @@
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
           <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>152400</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>15240</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>609600</xdr:colOff>
+      <xdr:row>33</xdr:row>
+      <xdr:rowOff>116840</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="图表 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{8512DA20-BAAB-424E-BE62-B3B3CAE4693C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
         </a:graphicData>
       </a:graphic>
     </xdr:graphicFrame>
@@ -1577,7 +2465,7 @@
   <dimension ref="A1:O31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="125" workbookViewId="0">
-      <selection activeCell="D33" sqref="D33"/>
+      <selection activeCell="L23" sqref="L23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16"/>
@@ -2127,7 +3015,13 @@
     </row>
     <row r="31" spans="1:14">
       <c r="B31">
-        <v>0.26132300000000003</v>
+        <v>261.32300000000004</v>
+      </c>
+      <c r="C31">
+        <v>400.41900000000004</v>
+      </c>
+      <c r="D31">
+        <v>460.11900000000003</v>
       </c>
     </row>
   </sheetData>

</xml_diff>